<commit_message>
Fixed 2 errors (#139 and #194) where the medical school years were not entered in the spreadsheet.
Updates the excel file to reflect changes made in the CSV.

Confirmed that #30 and #76 did not enter a medical school year.
</commit_message>
<xml_diff>
--- a/SurveyResponses.xlsx
+++ b/SurveyResponses.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SurveyResponses.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -127,26 +127,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,33 +153,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,15 +491,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI63" sqref="AI63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="560" topLeftCell="A10" activePane="bottomLeft"/>
+      <selection activeCell="P1" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:34">
       <c r="A1" t="s">
@@ -6433,7 +6395,7 @@
         <v>1</v>
       </c>
       <c r="AF59">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG59">
         <v>1</v>
@@ -14547,6 +14509,9 @@
       <c r="AC140">
         <v>1</v>
       </c>
+      <c r="AD140">
+        <v>3</v>
+      </c>
       <c r="AE140">
         <v>0</v>
       </c>
@@ -16246,25 +16211,25 @@
         <v>3</v>
       </c>
       <c r="G158">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H158">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I158">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J158">
         <v>4</v>
       </c>
       <c r="K158">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L158">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M158">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N158">
         <v>1</v>
@@ -16273,19 +16238,19 @@
         <v>1</v>
       </c>
       <c r="P158">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q158">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R158">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S158">
         <v>2</v>
       </c>
       <c r="T158">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U158">
         <v>1</v>
@@ -16306,15 +16271,18 @@
         <v>1</v>
       </c>
       <c r="AA158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB158">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC158">
         <v>1</v>
       </c>
       <c r="AD158">
+        <v>1</v>
+      </c>
+      <c r="AE158">
         <v>0</v>
       </c>
       <c r="AG158">
@@ -19898,6 +19866,9 @@
       <c r="C195">
         <v>3</v>
       </c>
+      <c r="D195">
+        <v>2</v>
+      </c>
       <c r="E195">
         <v>2</v>
       </c>
@@ -19905,46 +19876,46 @@
         <v>2</v>
       </c>
       <c r="G195">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H195">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I195">
         <v>2</v>
       </c>
       <c r="J195">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K195">
         <v>3</v>
       </c>
       <c r="L195">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M195">
         <v>2</v>
       </c>
       <c r="N195">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O195">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P195">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q195">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R195">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S195">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T195">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U195">
         <v>2</v>
@@ -19965,21 +19936,18 @@
         <v>2</v>
       </c>
       <c r="AA195">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB195">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AC195">
         <v>1</v>
       </c>
       <c r="AD195">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AE195">
-        <v>4</v>
-      </c>
-      <c r="AF195">
         <v>0</v>
       </c>
       <c r="AG195">
@@ -21174,7 +21142,7 @@
         <v>0</v>
       </c>
       <c r="AG207">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208" spans="1:34">
@@ -21782,7 +21750,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>